<commit_message>
raspberry pi ip port
</commit_message>
<xml_diff>
--- a/rest API.xlsx
+++ b/rest API.xlsx
@@ -98,7 +98,7 @@
     <t>emotion value in the past week</t>
   </si>
   <si>
-    <t>respberrypi-ip:172.29.92.105</t>
+    <t>respberrypi-ip:172.29.92.105:8888</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
correct the misspelling of restaurant
</commit_message>
<xml_diff>
--- a/rest API.xlsx
+++ b/rest API.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>play a song</t>
   </si>
@@ -59,9 +59,6 @@
     <t>/music?song=</t>
   </si>
   <si>
-    <t>/recommendation/restraunt</t>
-  </si>
-  <si>
     <t>/recommendation/music</t>
   </si>
   <si>
@@ -108,6 +105,15 @@
   </si>
   <si>
     <t>get a brightness</t>
+  </si>
+  <si>
+    <t>/recommendation/sports</t>
+  </si>
+  <si>
+    <t>get a recommendation of sports, return a list of sports (only 1 now)</t>
+  </si>
+  <si>
+    <t>/recommendation/restaurant</t>
   </si>
 </sst>
 </file>
@@ -427,9 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -440,18 +444,26 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -498,60 +510,60 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
         <v>21</v>
       </c>
-      <c r="B20" t="s">
-        <v>22</v>
-      </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
         <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed rest api recommendation of sports to 2
</commit_message>
<xml_diff>
--- a/rest API.xlsx
+++ b/rest API.xlsx
@@ -110,10 +110,10 @@
     <t>/recommendation/sports</t>
   </si>
   <si>
-    <t>get a recommendation of sports, return a list of sports (only 1 now)</t>
-  </si>
-  <si>
     <t>/recommendation/restaurant</t>
+  </si>
+  <si>
+    <t>get a recommendation of sports, return a list of sports (2 now)</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -444,7 +446,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -463,7 +465,7 @@
         <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>